<commit_message>
thought and preprocess half done
</commit_message>
<xml_diff>
--- a/result_schedule_2024_10_21.xlsx
+++ b/result_schedule_2024_10_21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/machine_1997/Desktop/mills_schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6815DA4D-3E59-EB43-8066-C0AE2495FC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E03C80-0AD2-8445-A51D-545B13B84CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="13880" xr2:uid="{5DAAE22D-AD04-AF49-BFB0-01E2E551B100}"/>
+    <workbookView xWindow="7500" yWindow="500" windowWidth="18020" windowHeight="13880" xr2:uid="{5DAAE22D-AD04-AF49-BFB0-01E2E551B100}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,10 +133,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,122 +474,122 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>